<commit_message>
Validaciones en carga masiva
</commit_message>
<xml_diff>
--- a/BDD/FORMATO_DE_CARGA_USUARIOS.xlsx
+++ b/BDD/FORMATO_DE_CARGA_USUARIOS.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
   <si>
     <t>NUM</t>
   </si>
@@ -430,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -520,12 +520,39 @@
         <v>16</v>
       </c>
     </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4">
+        <v>665544</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4">
+        <v>67890</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1"/>
     <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="E4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="271" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId3"/>
+  <pageSetup paperSize="271" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>